<commit_message>
Update file TienPhat(ra de cham)
</commit_message>
<xml_diff>
--- a/codeDaily/TienPhat.xlsx
+++ b/codeDaily/TienPhat.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>STT</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Day57</t>
+  </si>
+  <si>
+    <t>Day58</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +548,7 @@
         <v>107</v>
       </c>
       <c r="K4">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -573,11 +576,11 @@
       </c>
       <c r="K5">
         <f>SUM(K3+K4)</f>
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="L5">
         <f>SUM(J5+K5)</f>
-        <v>290</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -697,6 +700,21 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44446</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>